<commit_message>
added two class for industrial Questions
</commit_message>
<xml_diff>
--- a/Test Report/Report.xlsx
+++ b/Test Report/Report.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SiddharthM\eclipse\FCGA\Test Report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\New folder\FCGA-Version2\Test Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC070FEF-6B4E-452D-9B5E-17A2C8427515}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9135"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20700" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>TC ID</t>
   </si>
@@ -51,12 +52,24 @@
   </si>
   <si>
     <t>End Time</t>
+  </si>
+  <si>
+    <t>Class Description</t>
+  </si>
+  <si>
+    <t>Referral Reason</t>
+  </si>
+  <si>
+    <t>Class Code</t>
+  </si>
+  <si>
+    <t>Industial Question Count</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -397,26 +410,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.28515625" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="21" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="23.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="24.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="21" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="25.28515625" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="23.5703125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="24.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -427,25 +442,37 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -455,8 +482,12 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -466,8 +497,12 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -477,8 +512,12 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -488,8 +527,12 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -499,8 +542,12 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -510,8 +557,12 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -521,8 +572,12 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -532,8 +587,12 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -543,8 +602,12 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -554,8 +617,12 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -565,8 +632,12 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -576,8 +647,12 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -587,8 +662,12 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -598,8 +677,12 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -609,8 +692,12 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -620,6 +707,10 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>